<commit_message>
Added 2 new programs in python and their description
</commit_message>
<xml_diff>
--- a/Dataset/Characteristics.xlsx
+++ b/Dataset/Characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k2371605/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danif\Documents\GitHub\COW\XQuantum\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59350C2-50D1-D640-B408-5B899E9886F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F568486-4247-42C1-AE46-47ACC300B4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{A6814EC5-4716-6E4F-BF8A-321B4B4505A7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A6814EC5-4716-6E4F-BF8A-321B4B4505A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ae_indep_qiskit_5.qasm</t>
   </si>
@@ -111,6 +111,24 @@
   </si>
   <si>
     <t>Quantum walks are the quantum equivalent to classical random walks. In this no ancilla version, no ancilla qubits are used during its realization.</t>
+  </si>
+  <si>
+    <t>bell_state.py</t>
+  </si>
+  <si>
+    <t>ghz_state.py</t>
+  </si>
+  <si>
+    <t>Bell State</t>
+  </si>
+  <si>
+    <t>GHZ State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bell State entangles 2 qubits </t>
+  </si>
+  <si>
+    <t>GHZ State entangles 3 qubits</t>
   </si>
 </sst>
 </file>
@@ -178,11 +196,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -522,35 +539,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F3E87B2-58F5-524C-9BF7-D5D106928F6A}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="33" style="3" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="74.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,11 +577,11 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -574,11 +591,11 @@
       <c r="C3" s="1">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="92.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -588,11 +605,11 @@
       <c r="C4" s="1">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="37" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -602,11 +619,11 @@
       <c r="C5" s="1">
         <v>10</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -616,11 +633,11 @@
       <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="55.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -630,11 +647,11 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="37" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -644,8 +661,36 @@
       <c r="C8" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>